<commit_message>
revision plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1347 - CCOM, Martin Ochoa _MO/Planeación/Plan_proyecto.xlsx
+++ b/Proyectos/2015/11/P1347 - CCOM, Martin Ochoa _MO/Planeación/Plan_proyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,6 +31,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -158,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="177">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -265,6 +266,9 @@
     <t>Carta de aceptación</t>
   </si>
   <si>
+    <t>No recibida hasta la fecha</t>
+  </si>
+  <si>
     <t>Ciclo de Vida</t>
   </si>
   <si>
@@ -583,7 +587,7 @@
     <t>Frecuencia de monitoreo</t>
   </si>
   <si>
-    <t>Falla de conexión remota con Ammyy Admin En caso de fallar la conexión remota con Ammy Admin por no instalación o problemas de equipo</t>
+    <t>Falla de conexión remota con Ammyy Admin En caso de fallar la conexión remota con Ammy Admin por no instalación o problemas de equipo evita conexión con cliente</t>
   </si>
   <si>
     <t>TeamViwer, Show myPC</t>
@@ -598,7 +602,7 @@
     <t>Semanal</t>
   </si>
   <si>
-    <t>En caso de presentar problemas de instalación y configuración por problemas de compatibilidad</t>
+    <t>En caso de presentar problemas de instalación y configuración por problemas de compatibilidad puede romper el proyecto</t>
   </si>
   <si>
     <t>Validar los requerimientos minimos del equipo</t>
@@ -610,7 +614,7 @@
     <t>Ocurrido</t>
   </si>
   <si>
-    <t>Falla de descarga de programa ocasionada por una conexión a internet pobre o limitada</t>
+    <t>Falla de descarga de programa ocasionada por una conexión a internet pobre o limitada afecta tiempo de instalacion</t>
   </si>
   <si>
     <t>Validar que la descarga se halla realizado</t>
@@ -646,7 +650,7 @@
     <t>MA</t>
   </si>
   <si>
-    <t>No obtener carta de aceptación por un cliente que no contesta mensajes</t>
+    <t>No obtener carta de aceptación por un cliente que no contesta mensajes, afecta hito de cierre</t>
   </si>
   <si>
     <t>Enviar factura hasta obtener carta de aceptación</t>
@@ -1174,7 +1178,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1207,16 +1211,13 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="151">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1236,59 +1237,59 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1312,71 +1313,71 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1444,15 +1445,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1460,11 +1461,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1556,7 +1557,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1817,15 +1818,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1898,7 +1898,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2034,8 +2034,8 @@
   </sheetPr>
   <dimension ref="A1:AMI30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -4255,7 +4255,7 @@
         <v>42338</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>33</v>
       </c>
@@ -4265,7 +4265,9 @@
       <c r="C18" s="16" t="n">
         <v>42340</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A19" s="15"/>
@@ -4292,7 +4294,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="12"/>
@@ -4306,39 +4308,39 @@
     </row>
     <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="53.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B30" s="22"/>
     </row>
@@ -4396,7 +4398,7 @@
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24"/>
       <c r="B1" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -4404,7 +4406,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -4413,109 +4415,109 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C5" s="30" t="n">
         <v>3313482553</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="30" t="n">
         <v>3316367365</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C7" s="30" t="n">
         <v>3318039095</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>11</v>
@@ -4524,10 +4526,10 @@
         <v>3312448000</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4546,7 +4548,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
@@ -4555,19 +4557,19 @@
     </row>
     <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C13" s="34" t="n">
         <v>11369730</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4598,9 +4600,30 @@
       <c r="D17" s="37"/>
       <c r="E17" s="38"/>
     </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+    </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
@@ -4614,7 +4637,7 @@
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40"/>
       <c r="B23" s="41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -4659,19 +4682,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,10 +4702,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="46" t="n">
         <v>42340</v>
@@ -4764,8 +4787,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5862,7 +5885,7 @@
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="49" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -6889,19 +6912,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="50" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -7924,19 +7947,19 @@
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="51" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -8959,68 +8982,68 @@
     </row>
     <row r="5" s="56" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="54" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" s="56" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="54" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="55"/>
       <c r="C6" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" s="56" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" s="56" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" s="56" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9103,7 +9126,7 @@
     </row>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -9115,94 +9138,94 @@
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="58" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D4" s="36" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="60" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G4" s="36"/>
       <c r="J4" s="61" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="58" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D5" s="36" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="60" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G5" s="36"/>
       <c r="J5" s="61" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="62" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D6" s="59" t="n">
         <v>2</v>
       </c>
       <c r="E6" s="63"/>
       <c r="F6" s="63" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G6" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="61" t="s">
         <v>125</v>
-      </c>
-      <c r="J6" s="61" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9315,8 +9338,8 @@
   </sheetPr>
   <dimension ref="A1:JA43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9346,7 +9369,7 @@
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
       <c r="E2" s="68" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
@@ -9355,7 +9378,7 @@
       <c r="J2" s="69"/>
       <c r="K2" s="70"/>
       <c r="IR2" s="71" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="IS2" s="71"/>
       <c r="IT2" s="71"/>
@@ -9380,59 +9403,59 @@
       <c r="J3" s="75"/>
       <c r="K3" s="76"/>
       <c r="AE3" s="77" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AF3" s="77" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="78" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="79" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="80" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="80" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="81" t="s">
+        <v>140</v>
+      </c>
+      <c r="K4" s="80" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE4" s="82" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF4" s="82" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="79" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="80" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="80" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4" s="80" t="s">
-        <v>135</v>
-      </c>
-      <c r="G4" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="80" t="s">
-        <v>137</v>
-      </c>
-      <c r="I4" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="J4" s="81" t="s">
-        <v>139</v>
-      </c>
-      <c r="K4" s="80" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE4" s="82" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF4" s="82" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="83" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="84" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C5" s="83" t="n">
         <v>1</v>
@@ -9448,27 +9471,27 @@
         <v>4</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H5" s="84" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I5" s="86" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J5" s="87" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K5" s="88" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="83" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="84" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C6" s="83" t="n">
         <v>4</v>
@@ -9484,27 +9507,27 @@
         <v>3</v>
       </c>
       <c r="G6" s="84" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H6" s="88" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I6" s="86" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J6" s="87" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K6" s="88" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="83" t="n">
         <v>3</v>
       </c>
       <c r="B7" s="84" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C7" s="83" t="n">
         <v>4</v>
@@ -9520,19 +9543,19 @@
         <v>3</v>
       </c>
       <c r="G7" s="84" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H7" s="84" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I7" s="83" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J7" s="87" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K7" s="88" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9540,7 +9563,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C8" s="83" t="n">
         <v>5</v>
@@ -9556,19 +9579,19 @@
         <v>4</v>
       </c>
       <c r="G8" s="84" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H8" s="84" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I8" s="83" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="87" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K8" s="88" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="IS8" s="89"/>
       <c r="IT8" s="90"/>
@@ -9584,7 +9607,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="84" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C9" s="83" t="n">
         <v>5</v>
@@ -9600,25 +9623,25 @@
         <v>4</v>
       </c>
       <c r="G9" s="84" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H9" s="84" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I9" s="83" t="s">
         <v>11</v>
       </c>
       <c r="J9" s="87" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K9" s="88" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="IS9" s="94" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="IT9" s="95" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="IU9" s="96" t="n">
         <v>0.9</v>
@@ -9644,12 +9667,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="102" t="n">
         <v>6</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C10" s="83" t="n">
         <v>1</v>
@@ -9665,23 +9688,23 @@
         <v>3</v>
       </c>
       <c r="G10" s="84" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H10" s="84" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I10" s="83" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J10" s="87" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K10" s="88" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="IS10" s="94"/>
       <c r="IT10" s="95" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="IU10" s="96" t="n">
         <v>0.7</v>
@@ -9726,7 +9749,7 @@
       <c r="K11" s="110"/>
       <c r="IS11" s="94"/>
       <c r="IT11" s="95" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="IU11" s="96" t="n">
         <v>0.5</v>
@@ -9771,7 +9794,7 @@
       <c r="K12" s="110"/>
       <c r="IS12" s="94"/>
       <c r="IT12" s="95" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="IU12" s="96" t="n">
         <v>0.3</v>
@@ -9816,7 +9839,7 @@
       <c r="K13" s="110"/>
       <c r="IS13" s="94"/>
       <c r="IT13" s="95" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="IU13" s="117" t="n">
         <v>0.1</v>
@@ -9899,19 +9922,19 @@
       <c r="IT15" s="130"/>
       <c r="IU15" s="130"/>
       <c r="IV15" s="95" t="s">
+        <v>168</v>
+      </c>
+      <c r="IW15" s="95" t="s">
+        <v>169</v>
+      </c>
+      <c r="IX15" s="95" t="s">
+        <v>170</v>
+      </c>
+      <c r="IY15" s="95" t="s">
         <v>167</v>
       </c>
-      <c r="IW15" s="95" t="s">
-        <v>168</v>
-      </c>
-      <c r="IX15" s="95" t="s">
-        <v>169</v>
-      </c>
-      <c r="IY15" s="95" t="s">
-        <v>166</v>
-      </c>
       <c r="IZ15" s="132" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9935,7 +9958,7 @@
       <c r="IT16" s="130"/>
       <c r="IU16" s="96"/>
       <c r="IV16" s="133" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="IW16" s="133"/>
       <c r="IX16" s="133"/>
@@ -10012,7 +10035,7 @@
       <c r="J19" s="127"/>
       <c r="K19" s="128"/>
       <c r="IS19" s="137" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="IT19" s="137"/>
       <c r="IU19" s="135"/>
@@ -10040,12 +10063,12 @@
       <c r="J20" s="127"/>
       <c r="K20" s="128"/>
       <c r="IS20" s="138" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="IT20" s="139"/>
       <c r="IU20" s="135"/>
       <c r="IV20" s="140" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="IW20" s="140"/>
       <c r="IX20" s="140"/>
@@ -10070,12 +10093,12 @@
       <c r="J21" s="127"/>
       <c r="K21" s="128"/>
       <c r="IS21" s="138" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="IT21" s="141"/>
       <c r="IU21" s="135"/>
       <c r="IV21" s="140" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="IW21" s="140"/>
       <c r="IX21" s="140"/>
@@ -10100,12 +10123,12 @@
       <c r="J22" s="127"/>
       <c r="K22" s="128"/>
       <c r="IS22" s="138" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="IT22" s="142"/>
       <c r="IU22" s="135"/>
       <c r="IV22" s="140" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="IW22" s="140"/>
       <c r="IX22" s="140"/>

</xml_diff>